<commit_message>
Product backlog ja visual studio -projekti + vaatimusmaarittelyn alustavaa jakoa
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332004E4-A9F7-4448-AA80-CE7314ABF499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5C1A11-5D97-496D-8020-C96B01AA45CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>30 min</t>
+  </si>
+  <si>
+    <t>Tuntiseurantapohja, backlogin pohtimista</t>
+  </si>
+  <si>
+    <t>Planning, dokumentaatio</t>
   </si>
 </sst>
 </file>
@@ -582,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A3C75-48D6-4524-B97A-2F464AA41E3A}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,14 +635,26 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="11">
+        <v>44970</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="11">
+        <v>44974</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
@@ -789,7 +807,7 @@
       </c>
       <c r="B38" s="7">
         <f>SUM(B7:B37)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="C38" s="9"/>
     </row>
@@ -806,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755ADA5-B9A2-4F9F-B003-075794B7ABE1}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Vaatimusmäärittelydok.luvut 1 ja 4 täydennystä
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862315AF-5927-4217-80EA-60FFB92928BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F169888E-99EE-4785-A1BF-55E3F2A74DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Vaatimusmäärittely tietokanta</t>
+  </si>
+  <si>
+    <t>Vaatimusmäärittelydok., luvut 1 ja 4</t>
+  </si>
+  <si>
+    <t>Vaatimusmäärittelydok., luvut 1 ja 4; ulkoasun pohtimista</t>
   </si>
 </sst>
 </file>
@@ -575,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -585,26 +591,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A3C75-48D6-4524-B97A-2F464AA41E3A}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="3" max="3" width="45.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -612,15 +618,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -631,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>44970</v>
       </c>
@@ -642,7 +648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>44974</v>
       </c>
@@ -653,162 +659,174 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>44978</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>44979</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B38" s="7">
         <f>SUM(B7:B37)</f>
-        <v>1.25</v>
+        <v>2.25</v>
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -821,26 +839,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755ADA5-B9A2-4F9F-B003-075794B7ABE1}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="45.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -848,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -856,10 +874,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -870,7 +888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>44961</v>
       </c>
@@ -881,7 +899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>44973</v>
       </c>
@@ -892,7 +910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>44978</v>
       </c>
@@ -903,147 +921,147 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="14"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="14"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="14"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="14"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="14"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="14"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="14"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="14"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="14"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="14"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="14"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="14"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="14"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="14"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="14"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="14"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="14"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="14"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="14"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="14"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="14"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="14"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="14"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="14"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="14"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="14"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="14"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="14"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
@@ -1053,7 +1071,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -1070,22 +1088,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="3" max="3" width="45.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1093,15 +1111,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1112,162 +1130,162 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
@@ -1277,7 +1295,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Palaverimuistio 23022023 Sprint 2 planning
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DFD111-C7FB-4036-8D81-6AA4F78B1095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB20E30-DCF3-4802-A948-5B738AD92EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>0.5</t>
+  </si>
+  <si>
+    <t>Scrum-tiimin palavereja: daily, retro, review ja uuden sprintin planning.</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -594,26 +597,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A3C75-48D6-4524-B97A-2F464AA41E3A}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -621,15 +624,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -640,7 +643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>44970</v>
       </c>
@@ -651,7 +654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>44974</v>
       </c>
@@ -662,7 +665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>44978</v>
       </c>
@@ -673,7 +676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>44979</v>
       </c>
@@ -684,152 +687,158 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>44980</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B38" s="7">
         <f>SUM(B7:B37)</f>
-        <v>2.25</v>
+        <v>3.25</v>
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -842,26 +851,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755ADA5-B9A2-4F9F-B003-075794B7ABE1}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -869,7 +878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -877,10 +886,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -891,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>44961</v>
       </c>
@@ -902,7 +911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>44973</v>
       </c>
@@ -913,7 +922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>44978</v>
       </c>
@@ -924,7 +933,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>44979</v>
       </c>
@@ -935,142 +944,142 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="14"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="14"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="14"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="14"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="14"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="14"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="14"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="14"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="14"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="14"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="14"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="14"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="14"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="14"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="14"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="14"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="14"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="14"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="14"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="14"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="14"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="14"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="14"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="14"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="14"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="14"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="14"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1089,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>
@@ -1097,22 +1106,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1120,15 +1129,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1139,162 +1148,162 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
@@ -1304,7 +1313,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tyoajanseurannan ja product backlogin paivitys
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527B3FAB-5DDD-4AD6-B33D-A36461992B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BC3C6E-7552-4EB8-AA6D-9861D54F0C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Vaatimusmäärittely luku 7</t>
+  </si>
+  <si>
+    <t>CustomerWindow ja Customer-class toimintoja</t>
+  </si>
+  <si>
+    <t>Jaana Pusa</t>
   </si>
 </sst>
 </file>
@@ -677,7 +683,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,6 +713,9 @@
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -799,10 +808,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+    <row r="14" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <v>44986</v>
+      </c>
+      <c r="B14" s="5">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
@@ -925,7 +940,7 @@
       </c>
       <c r="B38" s="7">
         <f>SUM(B7:B37)</f>
-        <v>4.75</v>
+        <v>9.75</v>
       </c>
       <c r="C38" s="9"/>
     </row>

</xml_diff>

<commit_message>
Muokattu vaatimusmäärittelydokumentin muodoilua ja fiksattu Mainwindown ongelmat
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BC3C6E-7552-4EB8-AA6D-9861D54F0C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4BC49A-DEF4-42F4-8A06-B664F1384D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="33450" yWindow="1860" windowWidth="21630" windowHeight="11310" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Jaana Pusa</t>
+  </si>
+  <si>
+    <t>Scrum daily, retro, review ja planning</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,9 +823,15 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="10">
+        <v>44986</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
@@ -940,7 +949,7 @@
       </c>
       <c r="B38" s="7">
         <f>SUM(B7:B37)</f>
-        <v>9.75</v>
+        <v>10.25</v>
       </c>
       <c r="C38" s="9"/>
     </row>

</xml_diff>

<commit_message>
Mainwindow visuallook and Servicelevel
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4BC49A-DEF4-42F4-8A06-B664F1384D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23E1D5A-4CD7-48FD-9940-4D4A5F25C343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33450" yWindow="1860" windowWidth="21630" windowHeight="11310" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -122,12 +122,24 @@
   </si>
   <si>
     <t>Scrum daily, retro, review ja planning</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>Sprint-planning, Retroplanning</t>
+  </si>
+  <si>
+    <t>Serviceview ja MainWindow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -369,6 +381,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -675,7 +690,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A3C75-48D6-4524-B97A-2F464AA41E3A}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -966,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755ADA5-B9A2-4F9F-B003-075794B7ABE1}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,53 +1119,65 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="10">
+        <v>44986</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="10">
+        <v>44986</v>
+      </c>
+      <c r="B16" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
-      <c r="B19" s="12"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="12"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="12"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
-      <c r="B22" s="12"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="B23" s="12"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
-      <c r="B24" s="12"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1224,7 +1251,7 @@
       </c>
       <c r="B38" s="13">
         <f>SUM(B7:B37)</f>
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="C38" s="9"/>
     </row>

</xml_diff>

<commit_message>
Serviceview listbox add and removebutton
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A12DCDE-495D-4F09-8EC4-995B955B4260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F1EAB0-6244-41DC-A651-00BC465EA684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33450" yWindow="1860" windowWidth="21630" windowHeight="11310" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -130,10 +130,13 @@
     <t>Serviceview ja MainWindow</t>
   </si>
   <si>
-    <t>Pallvelutasot/kuukausihinnat</t>
-  </si>
-  <si>
     <t>Palvelutason saaminen json-tiedostosta CustomerWindown comboboxiin sekä korjauksia projektiin</t>
+  </si>
+  <si>
+    <t>Palvelutasot</t>
+  </si>
+  <si>
+    <t>Palvelutasot/kuukausihinnat</t>
   </si>
 </sst>
 </file>
@@ -693,7 +696,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -859,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -990,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755ADA5-B9A2-4F9F-B003-075794B7ABE1}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1157,13 +1160,19 @@
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="10">
+        <v>44988</v>
+      </c>
+      <c r="B18" s="24">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
@@ -1266,7 +1275,7 @@
       </c>
       <c r="B38" s="13">
         <f>SUM(B7:B37)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C38" s="9"/>
     </row>

</xml_diff>

<commit_message>
visual look, scrum daily
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEADF6E-D270-4C26-9AF2-0E638C09B922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20893630-0421-44F9-96F8-21F272313A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Listbox to listview, add class Invoice</t>
+  </si>
+  <si>
+    <t>Visuaalinen ilme, Scrum daily, service ja Customerwindow button lisäykset.</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1000,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F24" sqref="F23:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1188,10 +1191,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="5"/>
+    <row r="20" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10">
+        <v>44992</v>
+      </c>
+      <c r="B20" s="24">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
@@ -1284,7 +1293,7 @@
       </c>
       <c r="B38" s="13">
         <f>SUM(B7:B37)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C38" s="9"/>
     </row>

</xml_diff>

<commit_message>
Vaatimusmaarittelyn ja tyoajanseurannan paivitys
</commit_message>
<xml_diff>
--- a/Työajanseuranta/Tuntiseuranta.xlsx
+++ b/Työajanseuranta/Tuntiseuranta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lepi3\Documents\git\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaana\source\repos\Ohjelmistokehitysprojekti\Työajanseuranta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0273C9F6-2737-427D-9DA5-A60209E6ABB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52CDCFF-33A0-4A60-90EA-90B9A60EE08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{54EA30F5-A833-42E9-890A-E040A143837F}"/>
   </bookViews>
   <sheets>
     <sheet name="Jaana" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Työaikaraportti</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Vaatimusmäärittelu kohdat, Print ja retrokokokoukset</t>
+  </si>
+  <si>
+    <t>Koodikorjauksia Customer/Invoice</t>
+  </si>
+  <si>
+    <t>Dokumentaation päivitys, useamman asiakkaan laskujen näyttäminen listassa.</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -727,26 +733,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A3C75-48D6-4524-B97A-2F464AA41E3A}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -754,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -762,19 +768,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B5">
         <f>B39</f>
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -785,7 +791,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>44970</v>
       </c>
@@ -796,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>44974</v>
       </c>
@@ -807,7 +813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>44978</v>
       </c>
@@ -818,7 +824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>44979</v>
       </c>
@@ -829,7 +835,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>44982</v>
       </c>
@@ -840,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>44983</v>
       </c>
@@ -851,7 +857,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>44984</v>
       </c>
@@ -862,7 +868,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>44986</v>
       </c>
@@ -873,7 +879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>44986</v>
       </c>
@@ -884,7 +890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>44987</v>
       </c>
@@ -895,7 +901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>44992</v>
       </c>
@@ -906,117 +912,129 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>44994</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>44995</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="7">
         <f>SUM(B8:B38)</f>
-        <v>16.25</v>
+        <v>20.25</v>
       </c>
       <c r="C39" s="9"/>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
   </sheetData>
@@ -1029,26 +1047,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B755ADA5-B9A2-4F9F-B003-075794B7ABE1}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1056,7 +1074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1064,7 +1082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1073,10 +1091,10 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1087,7 +1105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>44961</v>
       </c>
@@ -1098,7 +1116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>44973</v>
       </c>
@@ -1109,7 +1127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>44974</v>
       </c>
@@ -1120,7 +1138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>44978</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>44979</v>
       </c>
@@ -1142,7 +1160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>44980</v>
       </c>
@@ -1153,7 +1171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>44981</v>
       </c>
@@ -1164,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>44984</v>
       </c>
@@ -1175,7 +1193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>44986</v>
       </c>
@@ -1186,7 +1204,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>44986</v>
       </c>
@@ -1197,7 +1215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>44987</v>
       </c>
@@ -1208,7 +1226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>44988</v>
       </c>
@@ -1219,7 +1237,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>44989</v>
       </c>
@@ -1230,7 +1248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>44990</v>
       </c>
@@ -1241,7 +1259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10">
         <v>44992</v>
       </c>
@@ -1252,7 +1270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>44993</v>
       </c>
@@ -1263,7 +1281,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>44994</v>
       </c>
@@ -1274,77 +1292,77 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="24"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="12"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="12"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="12"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="12"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="12"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="12"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="12"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="12"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="12"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="12"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="12"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="12"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="12"/>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>6</v>
       </c>
@@ -1354,7 +1372,7 @@
       </c>
       <c r="C39" s="9"/>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
   </sheetData>
@@ -1371,22 +1389,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1394,15 +1412,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1413,162 +1431,162 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" ht="31.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
@@ -1578,7 +1596,7 @@
       </c>
       <c r="C38" s="9"/>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
   </sheetData>

</xml_diff>